<commit_message>
Added inverted JLink adapter. First working code.
</commit_message>
<xml_diff>
--- a/Hardware/NFC_Toy_KiCAD/NFC_Toy.xlsx
+++ b/Hardware/NFC_Toy_KiCAD/NFC_Toy.xlsx
@@ -1273,7 +1273,6 @@
   <dxfs count="6">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1289,6 +1288,7 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1325,13 +1325,13 @@
   <autoFilter ref="A1:H38"/>
   <tableColumns count="8">
     <tableColumn id="1" uniqueName="1" name="Id" queryTableFieldId="1"/>
-    <tableColumn id="2" uniqueName="2" name="Designator" queryTableFieldId="2" dataDxfId="0"/>
-    <tableColumn id="3" uniqueName="3" name="Package" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="2" uniqueName="2" name="Designator" queryTableFieldId="2" dataDxfId="5"/>
+    <tableColumn id="3" uniqueName="3" name="Package" queryTableFieldId="3" dataDxfId="4"/>
     <tableColumn id="4" uniqueName="4" name="Quantity" queryTableFieldId="4"/>
-    <tableColumn id="5" uniqueName="5" name="Designation" queryTableFieldId="5" dataDxfId="5"/>
-    <tableColumn id="6" uniqueName="6" name="Supplier and ref" queryTableFieldId="6" dataDxfId="4"/>
-    <tableColumn id="7" uniqueName="7" name="Column1" queryTableFieldId="7" dataDxfId="3"/>
-    <tableColumn id="8" uniqueName="8" name="_1" queryTableFieldId="8" dataDxfId="2"/>
+    <tableColumn id="5" uniqueName="5" name="Designation" queryTableFieldId="5" dataDxfId="3"/>
+    <tableColumn id="6" uniqueName="6" name="Supplier and ref" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="7" uniqueName="7" name="Column1" queryTableFieldId="7" dataDxfId="1"/>
+    <tableColumn id="8" uniqueName="8" name="_1" queryTableFieldId="8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1637,15 +1637,15 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="81.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
@@ -2641,9 +2641,10 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>